<commit_message>
Updated Excel test data
</commit_message>
<xml_diff>
--- a/Excel/testdata.xlsx
+++ b/Excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\way2automation\PycharmProjects\PageObjectModelFramework\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rupali\PycharmProjects\POM_Selenium_Python\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD38B85-B024-488F-9C64-A3266C698AAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E343C9BA-A003-45BD-8BB6-1535BA464825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{9E2CB3D1-0571-491D-BF66-F783525DBCC6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9E2CB3D1-0571-491D-BF66-F783525DBCC6}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
@@ -49,24 +49,9 @@
     <t>password</t>
   </si>
   <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>trainer@way2automation.com</t>
-  </si>
-  <si>
     <t>India</t>
   </si>
   <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>rahularora1985</t>
-  </si>
-  <si>
-    <t>lsajdfksf</t>
-  </si>
-  <si>
     <t>carBrand</t>
   </si>
   <si>
@@ -95,6 +80,21 @@
   </si>
   <si>
     <t>BMW Cars</t>
+  </si>
+  <si>
+    <t>Mayank</t>
+  </si>
+  <si>
+    <t>mayank@mail.com</t>
+  </si>
+  <si>
+    <t>Lucknow</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -459,13 +459,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE81F5A-2F0A-4CDA-9E6E-3C1C5AF19B90}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,32 +491,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>3564684635</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>8927342</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{36FCE5A6-D847-4BBF-818F-16FAC5DAF989}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{91E26A61-353F-40C6-A36B-B6064FE34590}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -523,50 +526,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31209CD-93B8-4CBE-97B4-1AD94EFBB0DE}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>